<commit_message>
Documentos de primer avance
</commit_message>
<xml_diff>
--- a/Propuesta/Proyecto-Condensado-Equipo3 - corrección.xlsx
+++ b/Propuesta/Proyecto-Condensado-Equipo3 - corrección.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upbeduco-my.sharepoint.com/personal/angela_remolina_2019_upb_edu_co/Documents/Attachments/Proyecto integrador 2021-20/Propuesta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_69EF4EA411E5AE7F303CFB3B586F84D7D7BA5E2D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7944F1AD-3BF2-4A40-B5F1-773DF563227D}"/>
+  <xr:revisionPtr revIDLastSave="228" documentId="11_69EF4EA411E5AE7F303CFB3B586F84D7D7BA5E2D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BFE05D7-6B88-4714-8964-158676C051CA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
   <si>
     <t>FORMATO CONDENSADO DEL PROYECTO DE AULA / INTEGRADOR</t>
   </si>
@@ -160,13 +160,22 @@
   </si>
   <si>
     <t>NetBy</t>
+  </si>
+  <si>
+    <t>Terminado</t>
+  </si>
+  <si>
+    <t>No terminado</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,16 +240,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -673,11 +706,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -748,6 +855,69 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -757,19 +927,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -793,51 +951,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -856,14 +969,58 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="37" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="38" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="39" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="37" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="36" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="38" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="2" borderId="41" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="41" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bueno" xfId="1" builtinId="26"/>
+    <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1145,10 +1302,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G23"/>
+  <dimension ref="B1:I23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="101" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,88 +1313,103 @@
     <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="51.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="21" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="21" style="1" customWidth="1"/>
+    <col min="9" max="9" width="37" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="39" t="s">
+    <row r="1" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="41"/>
-    </row>
-    <row r="2" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
+    </row>
+    <row r="2" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="2:7" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="44"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="33"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="38"/>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
-    </row>
-    <row r="6" spans="2:7" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
+    </row>
+    <row r="6" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
-    </row>
-    <row r="7" spans="2:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
+    </row>
+    <row r="7" spans="2:9" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
-    </row>
-    <row r="8" spans="2:7" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+    </row>
+    <row r="8" spans="2:9" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
         <v>8</v>
       </c>
@@ -1253,12 +1425,18 @@
       <c r="F8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="54" t="s">
+    <row r="9" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="56" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="13" t="s">
@@ -1267,42 +1445,54 @@
       <c r="D9" s="14">
         <v>1</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="24">
         <v>44235</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="71"/>
+      <c r="I9" s="58" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
+    <row r="10" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="57"/>
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="57"/>
-    </row>
-    <row r="11" spans="2:7" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="58"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="73"/>
+      <c r="I10" s="59"/>
+    </row>
+    <row r="11" spans="2:9" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="60"/>
       <c r="C11" s="15" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
       </c>
-      <c r="E11" s="60"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="59"/>
-    </row>
-    <row r="12" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="54" t="s">
+      <c r="E11" s="28"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="67"/>
+      <c r="I11" s="61"/>
+    </row>
+    <row r="12" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="56" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="13" t="s">
@@ -1311,31 +1501,39 @@
       <c r="D12" s="14">
         <v>1</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="24">
         <f>F9</f>
         <v>44235</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="24">
         <v>44264</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="70" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="71"/>
+      <c r="I12" s="58" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="55"/>
+    <row r="13" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="57"/>
       <c r="C13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="57"/>
-    </row>
-    <row r="14" spans="2:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="54" t="s">
+      <c r="E13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="68"/>
+      <c r="I13" s="59"/>
+    </row>
+    <row r="14" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="56" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="13" t="s">
@@ -1344,31 +1542,39 @@
       <c r="D14" s="14">
         <v>2</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="24">
         <f>F12</f>
         <v>44264</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="56" t="s">
+      <c r="G14" s="74"/>
+      <c r="H14" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" s="58" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="55"/>
+    <row r="15" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="57"/>
       <c r="C15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="57"/>
-    </row>
-    <row r="16" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="54" t="s">
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="59"/>
+    </row>
+    <row r="16" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="56" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="13" t="s">
@@ -1377,31 +1583,39 @@
       <c r="D16" s="14">
         <v>1</v>
       </c>
-      <c r="E16" s="30" t="str">
+      <c r="E16" s="29" t="str">
         <f>F14</f>
         <v>17/09/2021</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="24">
         <v>44296</v>
       </c>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="70"/>
+      <c r="H16" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" s="58" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="55"/>
+    <row r="17" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="57"/>
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D17" s="5">
         <v>2</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="57"/>
-    </row>
-    <row r="18" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="68" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" s="59"/>
+    </row>
+    <row r="18" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="45" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -1410,85 +1624,101 @@
       <c r="D18" s="20">
         <v>1</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="24">
         <f>F16</f>
         <v>44296</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="G18" s="74"/>
+      <c r="H18" s="75" t="s">
+        <v>44</v>
+      </c>
+      <c r="I18" s="16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
+    <row r="19" spans="2:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="46"/>
       <c r="C19" s="21" t="s">
         <v>36</v>
       </c>
       <c r="D19" s="22">
         <v>1</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="33" t="s">
+      <c r="E19" s="25"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="50" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
+    <row r="20" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="46"/>
       <c r="C20" s="21" t="s">
         <v>39</v>
       </c>
       <c r="D20" s="17">
         <v>0.5</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="34"/>
-    </row>
-    <row r="21" spans="2:7" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="26"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="77" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="51"/>
+    </row>
+    <row r="21" spans="2:9" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="47"/>
       <c r="C21" s="23" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="18">
         <v>0.5</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="69" t="s">
+        <v>44</v>
+      </c>
+      <c r="I21" s="52"/>
+    </row>
+    <row r="22" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C6:I6"/>
     <mergeCell ref="F9:F11"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="E9:E11"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -1498,6 +1728,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006AEE2F69673B744B9A63162849AF731D" ma:contentTypeVersion="0" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="62ea272b3fbaa37195cbb92c300032c8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b2b1fa7a59e354d7f595b7732424404">
     <xsd:element name="properties">
@@ -1611,33 +1856,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C4D4A5E-78AA-4BA2-ACED-BA2245422AE8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EECF6E7E-5C9D-4900-A04D-6F91D8031B7B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1652,9 +1874,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EECF6E7E-5C9D-4900-A04D-6F91D8031B7B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C4D4A5E-78AA-4BA2-ACED-BA2245422AE8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>